<commit_message>
Updates for QA errors
Will run IG publisher on personal computer
</commit_message>
<xml_diff>
--- a/temp/pages/StructureDefinition-rtlsDevice.xlsx
+++ b/temp/pages/StructureDefinition-rtlsDevice.xlsx
@@ -63,7 +63,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-06-25T12:47:47-05:00</t>
+    <t>2025-07-29T13:31:52-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1524,17 +1524,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="31.41796875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="31.41796875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="9.79296875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="33.26953125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="5.30078125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="3.953125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="4.265625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="12.6875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="10.51171875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="32.75390625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="32.75390625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="9.984375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="34.9375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.29296875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.21484375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.55078125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.1171875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="10.75390625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="54.98046875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="57.3046875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1543,25 +1543,25 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="7.80078125" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="13.609375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="13.91796875" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="15.01171875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="7.93359375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="14.08984375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="14.4296875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="15.31640625" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="14.62890625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="34.984375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="41.32421875" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="17.98046875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="16.2578125" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="13.54296875" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="11.3203125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="28.8359375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="8.22265625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="8.53125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="36.796875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="42.97265625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.10546875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="17.6953125" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="15.98046875" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="13.44140625" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="11.03515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="30.5546875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="8.51953125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="8.859375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="50.1875" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="28.5078125" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="225.109375" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="52.78515625" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="29.45703125" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="234.19140625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>